<commit_message>
rfe: sort results by package name
</commit_message>
<xml_diff>
--- a/testdata/samples/bundles/xls/bundles_registry.redhat.io_redhat_certified_operator_index_v4.8_2021-05-14.xlsx
+++ b/testdata/samples/bundles/xls/bundles_registry.redhat.io_redhat_certified_operator_index_v4.8_2021-05-14.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
   <si>
     <t>Audit Bundle Report (Generated at 2021-05-14)</t>
   </si>
@@ -37,130 +37,130 @@
     <t>sha256:414ec051c4eec31a9f8e0e51eb4e0aa92653ca6b1d1c3da6cef92cb4bd21d0ed</t>
   </si>
   <si>
+    <t>Capabilities</t>
+  </si>
+  <si>
+    <t>Maintainer Name(s)</t>
+  </si>
+  <si>
+    <t>Operator Bundle Name</t>
+  </si>
+  <si>
+    <t>Has webhooks?</t>
+  </si>
+  <si>
+    <t>Project Layout</t>
+  </si>
+  <si>
+    <t>Scorecard Failing Tests</t>
+  </si>
+  <si>
     <t>Scorecard Suggestions</t>
   </si>
   <si>
+    <t>Maturity</t>
+  </si>
+  <si>
+    <t>Infrastructure</t>
+  </si>
+  <si>
+    <t>Has v1beta1 CRD?</t>
+  </si>
+  <si>
+    <t>Build At</t>
+  </si>
+  <si>
+    <t>Bundle Path</t>
+  </si>
+  <si>
+    <t>Validator Errors</t>
+  </si>
+  <si>
+    <t>Skips</t>
+  </si>
+  <si>
+    <t>Supports Multi Namespaces</t>
+  </si>
+  <si>
+    <t>Certified</t>
+  </si>
+  <si>
+    <t>Skip Range</t>
+  </si>
+  <si>
+    <t>Replace</t>
+  </si>
+  <si>
+    <t>Multiple Architectures</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>Default Channel</t>
+  </si>
+  <si>
+    <t>Scorecard Errors</t>
+  </si>
+  <si>
+    <t>Invalid Versioning</t>
+  </si>
+  <si>
+    <t>Supports Own Namespaces</t>
+  </si>
+  <si>
     <t>Repository</t>
   </si>
   <si>
-    <t>Certified</t>
-  </si>
-  <si>
-    <t>Bundle Path</t>
-  </si>
-  <si>
-    <t>Has webhooks?</t>
-  </si>
-  <si>
-    <t>Project Layout</t>
+    <t>Has possible performance issues</t>
+  </si>
+  <si>
+    <t>Found Replace</t>
+  </si>
+  <si>
+    <t>Maintainer Email(s)</t>
+  </si>
+  <si>
+    <t>Operator Bundle Version</t>
+  </si>
+  <si>
+    <t>Bundle Channel</t>
+  </si>
+  <si>
+    <t>Builder</t>
+  </si>
+  <si>
+    <t>Has Dependency</t>
+  </si>
+  <si>
+    <t>Supports All Namespaces</t>
+  </si>
+  <si>
+    <t>Package Name</t>
+  </si>
+  <si>
+    <t>SDK Version</t>
+  </si>
+  <si>
+    <t>Validator Warnings</t>
   </si>
   <si>
     <t>Invalid SkipRange</t>
   </si>
   <si>
-    <t>Has Dependency</t>
-  </si>
-  <si>
-    <t>Replace</t>
-  </si>
-  <si>
-    <t>Links</t>
-  </si>
-  <si>
-    <t>Has v1beta1 CRD?</t>
-  </si>
-  <si>
-    <t>Build At</t>
-  </si>
-  <si>
-    <t>SDK Version</t>
-  </si>
-  <si>
-    <t>Invalid Versioning</t>
-  </si>
-  <si>
-    <t>Supports Own Namespaces</t>
+    <t>Supports Single Namespaces</t>
   </si>
   <si>
     <t>OCP Labels Version</t>
   </si>
   <si>
-    <t>Maintainer Email(s)</t>
-  </si>
-  <si>
-    <t>Default Channel</t>
-  </si>
-  <si>
-    <t>Skips</t>
-  </si>
-  <si>
-    <t>Supports Multi Namespaces</t>
-  </si>
-  <si>
-    <t>Package Name</t>
-  </si>
-  <si>
-    <t>Scorecard Errors</t>
-  </si>
-  <si>
-    <t>Validator Errors</t>
-  </si>
-  <si>
-    <t>Validator Warnings</t>
-  </si>
-  <si>
-    <t>Supports Single Namespaces</t>
-  </si>
-  <si>
-    <t>Maturity</t>
-  </si>
-  <si>
-    <t>Multiple Architectures</t>
-  </si>
-  <si>
-    <t>Maintainer Name(s)</t>
-  </si>
-  <si>
-    <t>Infrastructure</t>
+    <t>Company</t>
   </si>
   <si>
     <t>Issues (To process this report)</t>
   </si>
   <si>
     <t>Categories</t>
-  </si>
-  <si>
-    <t>Operator Bundle Name</t>
-  </si>
-  <si>
-    <t>Bundle Channel</t>
-  </si>
-  <si>
-    <t>Scorecard Failing Tests</t>
-  </si>
-  <si>
-    <t>Found Replace</t>
-  </si>
-  <si>
-    <t>Operator Bundle Version</t>
-  </si>
-  <si>
-    <t>Builder</t>
-  </si>
-  <si>
-    <t>Skip Range</t>
-  </si>
-  <si>
-    <t>Supports All Namespaces</t>
-  </si>
-  <si>
-    <t>Capabilities</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Has possible performance issues</t>
   </si>
   <si>
     <t>alcide-kaudit-operator</t>
@@ -210,59 +210,60 @@
 olm-crds-have-resources</t>
   </si>
   <si>
-    <t>Add a spec descriptor for ingress
+    <t>Add a spec descriptor for k8s
+Add a spec descriptor for storage
+Add a spec descriptor for tls
+Add a spec descriptor for vault
+Add a spec descriptor for alcide
+Add a spec descriptor for aws
+Add a spec descriptor for resources
+Add a spec descriptor for aks
+Add a spec descriptor for kauditPolicyFile
+Add a spec descriptor for ingress
+Add a spec descriptor for runOptions
+Add a spec descriptor for image
 Add a spec descriptor for k8sAuditEnvironment
-Add a spec descriptor for resources
-Add a spec descriptor for vault
-Add a spec descriptor for storage
-Add a spec descriptor for aks
-Add a spec descriptor for alcide
 Add a spec descriptor for namespace
-Add a spec descriptor for aws
+Add a spec descriptor for prometheus
 Add a spec descriptor for clusterName
-Add a spec descriptor for image
-Add a spec descriptor for tls
 Add a spec descriptor for gke
-Add a spec descriptor for kauditPolicyFile
-Add a spec descriptor for prometheus
-Add a spec descriptor for runOptions
-Add CRD validation for spec field `gke` in Kaudit/v1alpha1
-Add CRD validation for spec field `storage` in Kaudit/v1alpha1
-Add CRD validation for spec field `resources` in Kaudit/v1alpha1
+Add CRD validation for spec field `k8s` in Kaudit/v1alpha1
+Add CRD validation for spec field `namespace` in Kaudit/v1alpha1
 Add CRD validation for spec field `aks` in Kaudit/v1alpha1
-Add CRD validation for spec field `alcide` in Kaudit/v1alpha1
 Add CRD validation for spec field `ingress` in Kaudit/v1alpha1
-Add CRD validation for spec field `kauditPolicyFile` in Kaudit/v1alpha1
-Add CRD validation for spec field `namespace` in Kaudit/v1alpha1
-Add CRD validation for spec field `prometheus` in Kaudit/v1alpha1
-Add CRD validation for spec field `vault` in Kaudit/v1alpha1
 Add CRD validation for spec field `tls` in Kaudit/v1alpha1
-Add CRD validation for spec field `aws` in Kaudit/v1alpha1
 Add CRD validation for spec field `clusterName` in Kaudit/v1alpha1
 Add CRD validation for spec field `image` in Kaudit/v1alpha1
-Add CRD validation for spec field `k8s` in Kaudit/v1alpha1
+Add CRD validation for spec field `kauditPolicyFile` in Kaudit/v1alpha1
+Add CRD validation for spec field `prometheus` in Kaudit/v1alpha1
+Add CRD validation for spec field `runOptions` in Kaudit/v1alpha1
+Add CRD validation for spec field `vault` in Kaudit/v1alpha1
+Add CRD validation for spec field `alcide` in Kaudit/v1alpha1
+Add CRD validation for spec field `gke` in Kaudit/v1alpha1
 Add CRD validation for spec field `k8sAuditEnvironment` in Kaudit/v1alpha1
-Add CRD validation for spec field `runOptions` in Kaudit/v1alpha1</t>
+Add CRD validation for spec field `resources` in Kaudit/v1alpha1
+Add CRD validation for spec field `storage` in Kaudit/v1alpha1
+Add CRD validation for spec field `aws` in Kaudit/v1alpha1</t>
   </si>
   <si>
     <t>kaudits.kaudit.alcide.com does not have a status descriptor
+k8s does not have a spec descriptor
+storage does not have a spec descriptor
+tls does not have a spec descriptor
+vault does not have a spec descriptor
+alcide does not have a spec descriptor
+aws does not have a spec descriptor
+resources does not have a spec descriptor
+aks does not have a spec descriptor
+kauditPolicyFile does not have a spec descriptor
 ingress does not have a spec descriptor
+runOptions does not have a spec descriptor
+image does not have a spec descriptor
 k8sAuditEnvironment does not have a spec descriptor
-resources does not have a spec descriptor
-vault does not have a spec descriptor
-storage does not have a spec descriptor
-aks does not have a spec descriptor
-alcide does not have a spec descriptor
-k8s does not have a spec descriptor
 namespace does not have a spec descriptor
-aws does not have a spec descriptor
+prometheus does not have a spec descriptor
 clusterName does not have a spec descriptor
-image does not have a spec descriptor
-tls does not have a spec descriptor
 gke does not have a spec descriptor
-kauditPolicyFile does not have a spec descriptor
-prometheus does not have a spec descriptor
-runOptions does not have a spec descriptor
 Owned CRDs do not have resources specified</t>
   </si>
   <si>
@@ -313,6 +314,81 @@
   </si>
   <si>
     <t>registry.connect.redhat.com/anaconda/anaconda-team-edition-bundle@sha256:43327356ec622d12126d5d13ae9c968dd7cc9e8555eadbb8e212d0b37cfb25a3</t>
+  </si>
+  <si>
+    <t>olm-spec-descriptors
+olm-status-descriptors
+olm-crds-have-resources</t>
+  </si>
+  <si>
+    <t>Add a spec descriptor for api
+Add a spec descriptor for dispatcher
+Add a spec descriptor for route
+Add a spec descriptor for postgres
+Add a spec descriptor for proxy
+Add a spec descriptor for redis
+Add a spec descriptor for storage
+Add a spec descriptor for worker
+Add CRD validation for spec field `worker` in AnacondaTeamEdition/v1beta1
+Add CRD validation for spec field `api` in AnacondaTeamEdition/v1beta1
+Add CRD validation for spec field `dispatcher` in AnacondaTeamEdition/v1beta1
+Add CRD validation for spec field `route` in AnacondaTeamEdition/v1beta1
+Add CRD validation for spec field `postgres` in AnacondaTeamEdition/v1beta1
+Add CRD validation for spec field `proxy` in AnacondaTeamEdition/v1beta1
+Add CRD validation for spec field `redis` in AnacondaTeamEdition/v1beta1
+Add CRD validation for spec field `storage` in AnacondaTeamEdition/v1beta1</t>
+  </si>
+  <si>
+    <t>api does not have a spec descriptor
+dispatcher does not have a spec descriptor
+route does not have a spec descriptor
+postgres does not have a spec descriptor
+proxy does not have a spec descriptor
+redis does not have a spec descriptor
+storage does not have a spec descriptor
+worker does not have a spec descriptor
+anacondateameditions.anaconda.com does not have a status descriptor
+Owned CRDs do not have resources specified</t>
+  </si>
+  <si>
+    <t>(anaconda-team-edition.v6.1.3) csv.Spec.Maintainers elements should contain both name and email</t>
+  </si>
+  <si>
+    <t>(anaconda-team-edition.v6.1.3) csv.Spec.minKubeVersion is not informed. It is recommended you provide this information. Otherwise, it would mean that your operator project can be distributed and installed in any cluster version available, which is not necessarily the case for all projects.
+apiextensions.k8s.io/v1beta1, kind=CustomResourceDefinitions was deprecated in Kubernetes v1.16 and will be removed in v1.22 in favor of v1: ["anacondateameditions.anaconda.com"] should be migrated</t>
+  </si>
+  <si>
+    <t>anchore-engine</t>
+  </si>
+  <si>
+    <t>https://github.com/anchore/engine-operator</t>
+  </si>
+  <si>
+    <t>https://www.anchore.com
+https://github.com/anchore/anchore-engine</t>
+  </si>
+  <si>
+    <t>Anchore Inc.</t>
+  </si>
+  <si>
+    <t>Brady Todhunter
+Zach Hill</t>
+  </si>
+  <si>
+    <t>bradyt@anchore.com
+zach@anchore.com</t>
+  </si>
+  <si>
+    <t>anchore-engine-operator.v0.1.11</t>
+  </si>
+  <si>
+    <t>0.1.11</t>
+  </si>
+  <si>
+    <t>2020-10-26T14:41:37.141641576Z</t>
+  </si>
+  <si>
+    <t>registry.connect.redhat.com/anchore/engine-operator-bundle@sha256:14066f319d8add2b868b13294bc6996ff119605fbc68736efcb8e9110a13110c</t>
   </si>
   <si>
     <t>olm-spec-descriptors
@@ -320,158 +396,27 @@
 olm-status-descriptors</t>
   </si>
   <si>
-    <t>Add a spec descriptor for proxy
-Add a spec descriptor for redis
-Add a spec descriptor for storage
-Add a spec descriptor for worker
-Add a spec descriptor for api
-Add a spec descriptor for dispatcher
-Add a spec descriptor for route
-Add a spec descriptor for postgres
-Add CRD validation for spec field `postgres` in AnacondaTeamEdition/v1beta1
-Add CRD validation for spec field `proxy` in AnacondaTeamEdition/v1beta1
-Add CRD validation for spec field `redis` in AnacondaTeamEdition/v1beta1
-Add CRD validation for spec field `storage` in AnacondaTeamEdition/v1beta1
-Add CRD validation for spec field `worker` in AnacondaTeamEdition/v1beta1
-Add CRD validation for spec field `api` in AnacondaTeamEdition/v1beta1
-Add CRD validation for spec field `dispatcher` in AnacondaTeamEdition/v1beta1
-Add CRD validation for spec field `route` in AnacondaTeamEdition/v1beta1</t>
-  </si>
-  <si>
-    <t>proxy does not have a spec descriptor
-redis does not have a spec descriptor
-storage does not have a spec descriptor
-worker does not have a spec descriptor
-api does not have a spec descriptor
-dispatcher does not have a spec descriptor
-route does not have a spec descriptor
-postgres does not have a spec descriptor
-Owned CRDs do not have resources specified
-anacondateameditions.anaconda.com does not have a status descriptor</t>
-  </si>
-  <si>
-    <t>(anaconda-team-edition.v6.1.3) csv.Spec.Maintainers elements should contain both name and email</t>
-  </si>
-  <si>
-    <t>(anaconda-team-edition.v6.1.3) csv.Spec.minKubeVersion is not informed. It is recommended you provide this information. Otherwise, it would mean that your operator project can be distributed and installed in any cluster version available, which is not necessarily the case for all projects.
-apiextensions.k8s.io/v1beta1, kind=CustomResourceDefinitions was deprecated in Kubernetes v1.16 and will be removed in v1.22 in favor of v1: ["anacondateameditions.anaconda.com"] should be migrated</t>
-  </si>
-  <si>
-    <t>appdynamics-operator</t>
-  </si>
-  <si>
-    <t>https://github.com/Appdynamics/appdynamics-operator</t>
-  </si>
-  <si>
-    <t>https://docs.appdynamics.com/display/PRO45/Monitoring+Kubernetes+with+the+Cluster+Agent
-https://www.appdynamics.com/cloud-monitoring/kubernetes-monitoring/
-https://github.com/Appdynamics/appdynamics-operator</t>
-  </si>
-  <si>
-    <t>Monitoring</t>
-  </si>
-  <si>
-    <t>AppDynamics LLC</t>
-  </si>
-  <si>
-    <t>AppDynamics</t>
-  </si>
-  <si>
-    <t>support@appdynamics.com</t>
-  </si>
-  <si>
-    <t>appdynamics-operator.v0.6.3</t>
-  </si>
-  <si>
-    <t>0.6.3</t>
-  </si>
-  <si>
-    <t>2020-11-04T10:19:30.592282909Z</t>
-  </si>
-  <si>
-    <t>registry.connect.redhat.com/appdynamics/cluster-agent-operator-bundle@sha256:cebac3376fe72321aefd39f816331f37242f602e1133ec2f6d825cc128a8d066</t>
-  </si>
-  <si>
-    <t>olm-spec-descriptors
-olm-status-descriptors</t>
-  </si>
-  <si>
-    <t>Add a spec descriptor for enableMasters
-Add a spec descriptor for netVizPort
-Add a spec descriptor for stdoutLogging
-Add a spec descriptor for enableDockerViz</t>
-  </si>
-  <si>
-    <t>enableMasters does not have a spec descriptor
-netVizPort does not have a spec descriptor
-stdoutLogging does not have a spec descriptor
-enableDockerViz does not have a spec descriptor
-adams.appdynamics.com does not have a status descriptor
-clusteragents.appdynamics.com does not have a status descriptor
-infravizs.appdynamics.com does not have a status descriptor</t>
-  </si>
-  <si>
-    <t>(appdynamics-operator.v0.6.3) csv.Spec.minKubeVersion is not informed. It is recommended you provide this information. Otherwise, it would mean that your operator project can be distributed and installed in any cluster version available, which is not necessarily the case for all projects.
-apiextensions.k8s.io/v1beta1, kind=CustomResourceDefinitions was deprecated in Kubernetes v1.16 and will be removed in v1.22 in favor of v1: ["adams.appdynamics.com" "clusteragents.appdynamics.com" "infravizs.appdynamics.com"] should be migrated</t>
-  </si>
-  <si>
-    <t>appdynamics-operator.v0.4.3</t>
-  </si>
-  <si>
-    <t>anchore-engine</t>
-  </si>
-  <si>
-    <t>https://github.com/anchore/engine-operator</t>
-  </si>
-  <si>
-    <t>https://www.anchore.com
-https://github.com/anchore/anchore-engine</t>
-  </si>
-  <si>
-    <t>Anchore Inc.</t>
-  </si>
-  <si>
-    <t>Brady Todhunter
-Zach Hill</t>
-  </si>
-  <si>
-    <t>bradyt@anchore.com
-zach@anchore.com</t>
-  </si>
-  <si>
-    <t>anchore-engine-operator.v0.1.11</t>
-  </si>
-  <si>
-    <t>0.1.11</t>
-  </si>
-  <si>
-    <t>2020-10-26T14:41:37.141641576Z</t>
-  </si>
-  <si>
-    <t>registry.connect.redhat.com/anchore/engine-operator-bundle@sha256:14066f319d8add2b868b13294bc6996ff119605fbc68736efcb8e9110a13110c</t>
-  </si>
-  <si>
-    <t>Add CRD validation for AnchoreEngine/v1alpha1
+    <t>Add a spec descriptor for anchorePolicyEngine
+Add a spec descriptor for anchoreSimpleQueue
+Add a spec descriptor for ingress
+Add a spec descriptor for postgresql
 Add a spec descriptor for anchoreAnalyzer
 Add a spec descriptor for anchoreApi
 Add a spec descriptor for anchoreCatalog
 Add a spec descriptor for anchoreGlobal
-Add a spec descriptor for anchorePolicyEngine
-Add a spec descriptor for anchoreSimpleQueue
-Add a spec descriptor for ingress
-Add a spec descriptor for postgresql</t>
-  </si>
-  <si>
-    <t>anchoreengines.anchore.com does not have a status descriptor
+Add CRD validation for AnchoreEngine/v1alpha1</t>
+  </si>
+  <si>
+    <t>anchorePolicyEngine does not have a spec descriptor
+anchoreSimpleQueue does not have a spec descriptor
+ingress does not have a spec descriptor
+postgresql does not have a spec descriptor
 anchoreAnalyzer does not have a spec descriptor
 anchoreApi does not have a spec descriptor
 anchoreCatalog does not have a spec descriptor
 anchoreGlobal does not have a spec descriptor
-anchorePolicyEngine does not have a spec descriptor
-anchoreSimpleQueue does not have a spec descriptor
-ingress does not have a spec descriptor
-postgresql does not have a spec descriptor
-Owned CRDs do not have resources specified</t>
+Owned CRDs do not have resources specified
+anchoreengines.anchore.com does not have a status descriptor</t>
   </si>
   <si>
     <t>(anchore-engine-operator.v0.1.11) csv.Spec.minKubeVersion is not informed. It is recommended you provide this information. Otherwise, it would mean that your operator project can be distributed and installed in any cluster version available, which is not necessarily the case for all projects.
@@ -513,6 +458,67 @@
   <si>
     <t>(anzo-operator.v1.1.103) csv.Spec.minKubeVersion is not informed. It is recommended you provide this information. Otherwise, it would mean that your operator project can be distributed and installed in any cluster version available, which is not necessarily the case for all projects.
 apiextensions.k8s.io/v1beta1, kind=CustomResourceDefinitions was deprecated in Kubernetes v1.16 and will be removed in v1.22 in favor of v1: ["anzos.anzo.cambridgesemantics.com"] should be migrated</t>
+  </si>
+  <si>
+    <t>appdynamics-operator</t>
+  </si>
+  <si>
+    <t>https://github.com/Appdynamics/appdynamics-operator</t>
+  </si>
+  <si>
+    <t>https://docs.appdynamics.com/display/PRO45/Monitoring+Kubernetes+with+the+Cluster+Agent
+https://www.appdynamics.com/cloud-monitoring/kubernetes-monitoring/
+https://github.com/Appdynamics/appdynamics-operator</t>
+  </si>
+  <si>
+    <t>Monitoring</t>
+  </si>
+  <si>
+    <t>AppDynamics LLC</t>
+  </si>
+  <si>
+    <t>AppDynamics</t>
+  </si>
+  <si>
+    <t>support@appdynamics.com</t>
+  </si>
+  <si>
+    <t>appdynamics-operator.v0.6.3</t>
+  </si>
+  <si>
+    <t>0.6.3</t>
+  </si>
+  <si>
+    <t>2020-11-04T10:19:30.592282909Z</t>
+  </si>
+  <si>
+    <t>registry.connect.redhat.com/appdynamics/cluster-agent-operator-bundle@sha256:cebac3376fe72321aefd39f816331f37242f602e1133ec2f6d825cc128a8d066</t>
+  </si>
+  <si>
+    <t>olm-status-descriptors
+olm-spec-descriptors</t>
+  </si>
+  <si>
+    <t>Add a spec descriptor for enableDockerViz
+Add a spec descriptor for enableMasters
+Add a spec descriptor for netVizPort
+Add a spec descriptor for stdoutLogging</t>
+  </si>
+  <si>
+    <t>adams.appdynamics.com does not have a status descriptor
+clusteragents.appdynamics.com does not have a status descriptor
+infravizs.appdynamics.com does not have a status descriptor
+enableDockerViz does not have a spec descriptor
+enableMasters does not have a spec descriptor
+netVizPort does not have a spec descriptor
+stdoutLogging does not have a spec descriptor</t>
+  </si>
+  <si>
+    <t>(appdynamics-operator.v0.6.3) csv.Spec.minKubeVersion is not informed. It is recommended you provide this information. Otherwise, it would mean that your operator project can be distributed and installed in any cluster version available, which is not necessarily the case for all projects.
+apiextensions.k8s.io/v1beta1, kind=CustomResourceDefinitions was deprecated in Kubernetes v1.16 and will be removed in v1.22 in favor of v1: ["adams.appdynamics.com" "clusteragents.appdynamics.com" "infravizs.appdynamics.com"] should be migrated</t>
+  </si>
+  <si>
+    <t>appdynamics-operator.v0.4.3</t>
   </si>
 </sst>
 </file>
@@ -925,130 +931,130 @@
     </row>
     <row r="5" ht="15" customHeight="true">
       <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="P5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>17</v>
+      </c>
+      <c r="R5" t="s">
+        <v>18</v>
+      </c>
+      <c r="S5" t="s">
+        <v>10</v>
+      </c>
+      <c r="T5" t="s">
         <v>37</v>
       </c>
-      <c r="G5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K5" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" t="s">
-        <v>38</v>
-      </c>
-      <c r="N5" t="s">
-        <v>42</v>
-      </c>
-      <c r="O5" t="s">
-        <v>24</v>
-      </c>
-      <c r="P5" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>18</v>
-      </c>
-      <c r="R5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S5" t="s">
+      <c r="U5" t="s">
+        <v>41</v>
+      </c>
+      <c r="V5" t="s">
         <v>11</v>
       </c>
-      <c r="T5" t="s">
-        <v>43</v>
-      </c>
-      <c r="U5" t="s">
-        <v>19</v>
-      </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>12</v>
       </c>
-      <c r="W5" t="s">
-        <v>40</v>
-      </c>
       <c r="X5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="Y5" t="s">
         <v>28</v>
       </c>
       <c r="Z5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB5" t="s">
         <v>29</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AC5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK5" t="s">
         <v>30</v>
       </c>
-      <c r="AB5" t="s">
-        <v>20</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>44</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AH5" t="s">
+      <c r="AL5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM5" t="s">
         <v>15</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AN5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AO5" t="s">
         <v>45</v>
       </c>
-      <c r="AJ5" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>21</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>26</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>35</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>48</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>22</v>
-      </c>
       <c r="AP5" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="true">
@@ -1324,31 +1330,31 @@
         <v>53</v>
       </c>
       <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" t="s">
         <v>90</v>
       </c>
-      <c r="G8" t="s">
-        <v>50</v>
-      </c>
-      <c r="H8" t="s">
-        <v>56</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>91</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>92</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>93</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>94</v>
-      </c>
-      <c r="N8" t="s">
-        <v>95</v>
       </c>
       <c r="O8" t="s">
         <v>52</v>
@@ -1357,37 +1363,37 @@
         <v>52</v>
       </c>
       <c r="Q8" t="s">
+        <v>95</v>
+      </c>
+      <c r="R8" t="s">
         <v>96</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
+        <v>55</v>
+      </c>
+      <c r="T8" t="s">
+        <v>50</v>
+      </c>
+      <c r="U8" t="s">
+        <v>50</v>
+      </c>
+      <c r="V8" t="s">
+        <v>50</v>
+      </c>
+      <c r="W8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="S8" t="s">
-        <v>55</v>
-      </c>
-      <c r="T8" t="s">
-        <v>50</v>
-      </c>
-      <c r="U8" t="s">
-        <v>50</v>
-      </c>
-      <c r="V8" t="s">
-        <v>50</v>
-      </c>
-      <c r="W8" s="2" t="s">
+      <c r="X8" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="X8" s="2" t="s">
+      <c r="Y8" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="Y8" s="2" t="s">
+      <c r="Z8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA8" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="Z8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA8" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="AB8" t="s">
         <v>55</v>
@@ -1405,7 +1411,7 @@
         <v>50</v>
       </c>
       <c r="AG8" t="s">
-        <v>102</v>
+        <v>50</v>
       </c>
       <c r="AH8" t="s">
         <v>50</v>
@@ -1437,22 +1443,22 @@
     </row>
     <row r="9" ht="15" customHeight="true">
       <c r="A9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" t="s">
         <v>103</v>
-      </c>
-      <c r="B9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9" t="s">
-        <v>52</v>
       </c>
       <c r="E9" t="s">
         <v>53</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>104</v>
       </c>
       <c r="G9" t="s">
         <v>50</v>
@@ -1464,58 +1470,58 @@
         <v>56</v>
       </c>
       <c r="J9" t="s">
+        <v>105</v>
+      </c>
+      <c r="K9" t="s">
         <v>106</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>107</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>108</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>109</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
+        <v>103</v>
+      </c>
+      <c r="P9" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q9" t="s">
         <v>110</v>
       </c>
-      <c r="O9" t="s">
-        <v>52</v>
-      </c>
-      <c r="P9" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>111</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
+        <v>55</v>
+      </c>
+      <c r="T9" t="s">
+        <v>50</v>
+      </c>
+      <c r="U9" t="s">
+        <v>50</v>
+      </c>
+      <c r="V9" t="s">
+        <v>50</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA9" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="S9" t="s">
-        <v>55</v>
-      </c>
-      <c r="T9" t="s">
-        <v>50</v>
-      </c>
-      <c r="U9" t="s">
-        <v>50</v>
-      </c>
-      <c r="V9" t="s">
-        <v>50</v>
-      </c>
-      <c r="W9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="X9" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y9" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="Z9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA9" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="AB9" t="s">
         <v>55</v>
@@ -1539,7 +1545,7 @@
         <v>50</v>
       </c>
       <c r="AI9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AJ9" t="s">
         <v>56</v>
@@ -1565,79 +1571,79 @@
     </row>
     <row r="10" ht="15" customHeight="true">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>114</v>
       </c>
       <c r="C10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
         <v>53</v>
       </c>
       <c r="F10" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" t="s">
+        <v>117</v>
+      </c>
+      <c r="K10" t="s">
+        <v>118</v>
+      </c>
+      <c r="L10" t="s">
         <v>119</v>
       </c>
-      <c r="G10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" t="s">
-        <v>56</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="M10" t="s">
         <v>120</v>
       </c>
-      <c r="K10" t="s">
+      <c r="N10" t="s">
         <v>121</v>
       </c>
-      <c r="L10" t="s">
+      <c r="O10" t="s">
+        <v>52</v>
+      </c>
+      <c r="P10" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q10" t="s">
         <v>122</v>
       </c>
-      <c r="M10" t="s">
+      <c r="R10" t="s">
         <v>123</v>
       </c>
-      <c r="N10" t="s">
+      <c r="S10" t="s">
+        <v>55</v>
+      </c>
+      <c r="T10" t="s">
+        <v>50</v>
+      </c>
+      <c r="U10" t="s">
+        <v>50</v>
+      </c>
+      <c r="V10" t="s">
+        <v>50</v>
+      </c>
+      <c r="W10" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="O10" t="s">
-        <v>118</v>
-      </c>
-      <c r="P10" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q10" t="s">
+      <c r="X10" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="R10" t="s">
+      <c r="Y10" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="S10" t="s">
-        <v>55</v>
-      </c>
-      <c r="T10" t="s">
-        <v>50</v>
-      </c>
-      <c r="U10" t="s">
-        <v>50</v>
-      </c>
-      <c r="V10" t="s">
-        <v>50</v>
-      </c>
-      <c r="W10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="X10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y10" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="Z10" s="2" t="s">
         <v>50</v>
@@ -1661,13 +1667,13 @@
         <v>50</v>
       </c>
       <c r="AG10" t="s">
-        <v>50</v>
+        <v>128</v>
       </c>
       <c r="AH10" t="s">
         <v>50</v>
       </c>
       <c r="AI10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AJ10" t="s">
         <v>56</v>

</xml_diff>